<commit_message>
Update survey data 2019
</commit_message>
<xml_diff>
--- a/data/2019/encuesta2019.xlsx
+++ b/data/2019/encuesta2019.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="10">
   <si>
     <t>fecha</t>
   </si>
@@ -60,8 +60,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,9 +97,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1525,63 +1534,225 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1">
+        <v>43486</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1">
+        <v>43486</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1">
+        <v>43486</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1">
+        <v>43486</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1">
+        <v>43486</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1">
+        <v>43486</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1">
+        <v>43486</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -1610,5 +1781,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>